<commit_message>
new added data for test
</commit_message>
<xml_diff>
--- a/bulk_mail/data/contacts.xlsx
+++ b/bulk_mail/data/contacts.xlsx
@@ -2,16 +2,18 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\python\apy35\bulk_mail\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Лист1!$A$1:$A$13</definedName>
-  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -22,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
   <si>
     <t>email</t>
   </si>
@@ -33,82 +35,46 @@
     <t>subject</t>
   </si>
   <si>
-    <t>body_plain</t>
-  </si>
-  <si>
     <t>body_html</t>
   </si>
   <si>
-    <t>salutation_plain</t>
-  </si>
-  <si>
-    <t>signature_plain</t>
-  </si>
-  <si>
     <t>salutation_html</t>
   </si>
   <si>
     <t>signature_html</t>
   </si>
   <si>
-    <t>apy35test+p1@gmail.com</t>
-  </si>
-  <si>
-    <t>apy35test+p2@gmail.com</t>
-  </si>
-  <si>
-    <t>apy35test+p3@gmail.com</t>
-  </si>
-  <si>
-    <t>apy35test+p4@gmail.com</t>
-  </si>
-  <si>
-    <t>halkaFulka</t>
+    <t>kill bill</t>
+  </si>
+  <si>
+    <t>Invoice from Jack's Store</t>
+  </si>
+  <si>
+    <t>apy35hot11_test@hotmail.com</t>
+  </si>
+  <si>
+    <t>body_html.txt</t>
+  </si>
+  <si>
+    <t>body_html1.txt</t>
+  </si>
+  <si>
+    <t>salutation_html.txt</t>
+  </si>
+  <si>
+    <t>salutation_html1.txt</t>
+  </si>
+  <si>
+    <t>signature_html.txt</t>
+  </si>
+  <si>
+    <t>signature_html1.txt</t>
   </si>
   <si>
     <t>iitbguha@gmail.com</t>
   </si>
   <si>
-    <t>apy35_test@outlook.com</t>
-  </si>
-  <si>
-    <t>anjani_test@outlook.com</t>
-  </si>
-  <si>
-    <t>apy35hot_test@hotmail.com</t>
-  </si>
-  <si>
-    <t>Invoice from Jack's Store</t>
-  </si>
-  <si>
-    <t>Did I get something wrong</t>
-  </si>
-  <si>
-    <t>invoicing you to Twitter</t>
-  </si>
-  <si>
-    <t>kill bill</t>
-  </si>
-  <si>
-    <t>naruto</t>
-  </si>
-  <si>
-    <t>sasuke</t>
-  </si>
-  <si>
-    <t>sasuke uchiha</t>
-  </si>
-  <si>
-    <t>uchiha</t>
-  </si>
-  <si>
-    <t>sasuke sas</t>
-  </si>
-  <si>
-    <t>naruto oro</t>
-  </si>
-  <si>
-    <t>naruto oka</t>
+    <t>iitbguha+p1@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -444,26 +410,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.33203125" customWidth="1"/>
-    <col min="4" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -477,168 +440,78 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+      <c r="E4" t="s">
         <v>11</v>
       </c>
-      <c r="B10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+      <c r="F4" t="s">
         <v>13</v>
-      </c>
-      <c r="B11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A9" r:id="rId3"/>
-    <hyperlink ref="A6" r:id="rId4"/>
-    <hyperlink ref="A10" r:id="rId5"/>
-    <hyperlink ref="A12" r:id="rId6"/>
-    <hyperlink ref="A8" r:id="rId7"/>
-    <hyperlink ref="A11" r:id="rId8" display="apyhot_test+p4@hotmail.com"/>
-    <hyperlink ref="A4" r:id="rId9"/>
-    <hyperlink ref="A7" r:id="rId10"/>
-    <hyperlink ref="A13" r:id="rId11"/>
+    <hyperlink ref="A4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>